<commit_message>
20150107 - Updated Manual Derivative Matrix Excel
Updated Excel sheet with new balance equation derivatives.
</commit_message>
<xml_diff>
--- a/Matrix Dependence.xlsx
+++ b/Matrix Dependence.xlsx
@@ -11,12 +11,13 @@
     <sheet name="Matrix by Hand" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_20141222_Matrix" localSheetId="1">'Matrix by Hand'!$D$36:$K$43</definedName>
+    <definedName name="_20141222_Matrix" localSheetId="1">'Matrix by Hand'!#REF!</definedName>
     <definedName name="air">'Matrix by Hand'!$B$14</definedName>
     <definedName name="Cp_a">'Matrix by Hand'!$B$9</definedName>
     <definedName name="Cp_w">'Matrix by Hand'!$B$8</definedName>
     <definedName name="m_a">'Matrix by Hand'!$B$7</definedName>
     <definedName name="m_w">'Matrix by Hand'!$B$6</definedName>
+    <definedName name="ManualDerivativeMatrix" localSheetId="1">'Matrix by Hand'!$D$36:$K$43</definedName>
     <definedName name="R_ext">'Matrix by Hand'!$B$12</definedName>
     <definedName name="R_int">'Matrix by Hand'!$B$11</definedName>
     <definedName name="R_pipe">'Matrix by Hand'!$B$10</definedName>
@@ -54,11 +55,25 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="ManualDerivativeMatrix.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:justinshultz:Dropbox:ICSolarThermalModel:Supporting Material:ManualDerivativeMatrix.txt" delimited="0">
+      <textFields count="8">
+        <textField/>
+        <textField position="15"/>
+        <textField position="32"/>
+        <textField position="49"/>
+        <textField position="66"/>
+        <textField position="83"/>
+        <textField position="101"/>
+        <textField position="118"/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="58">
   <si>
     <t>x</t>
   </si>
@@ -195,27 +210,9 @@
     <t>m_a*Cp_a</t>
   </si>
   <si>
-    <t>-m_w*Cp_w*1+1/2/R_pipe</t>
-  </si>
-  <si>
-    <t>1/2/R_pipe</t>
-  </si>
-  <si>
-    <t>-1/2/R_pipe</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
-    <t>m_w*Cp_w*1+1/2/R_pipe</t>
-  </si>
-  <si>
-    <t>-m_a*Cp_a+1/2/R_pipe+1/2/R_int+1/2/R_ext</t>
-  </si>
-  <si>
-    <t>m_a*Cp_a+1/2/R_pipe+1/2/R_int+1/2/R_ext</t>
-  </si>
-  <si>
     <t>-m_w*Cp_w</t>
   </si>
   <si>
@@ -238,13 +235,65 @@
   </si>
   <si>
     <t>F2</t>
+  </si>
+  <si>
+    <r>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="205"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>m_w</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="206"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cp_w</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*1</t>
+    </r>
+  </si>
+  <si>
+    <t>m_w*Cp_w*1+1/R_pipe</t>
+  </si>
+  <si>
+    <t>-1/R_pipe</t>
+  </si>
+  <si>
+    <t>m_a*Cp_a+1/R_pipe+1/R_int+1/R_ext</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,8 +325,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="205"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="206"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,8 +363,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -311,8 +378,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -340,20 +422,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -367,6 +461,10 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -380,6 +478,10 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -436,8 +538,8 @@
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>325120</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
@@ -491,8 +593,8 @@
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -547,7 +649,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>477520</xdr:colOff>
+      <xdr:colOff>248920</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
@@ -597,7 +699,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="20141222_Matrix" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ManualDerivativeMatrix" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -855,7 +957,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1370,15 +1472,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="13.1640625" customWidth="1"/>
+    <col min="2" max="11" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1529,34 +1629,34 @@
         <v>1</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1564,34 +1664,34 @@
         <v>2</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1599,34 +1699,34 @@
         <v>3</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1634,34 +1734,34 @@
         <v>4</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>44</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1669,34 +1769,34 @@
         <v>15</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J21" s="6">
-        <v>0</v>
-      </c>
-      <c r="K21" s="6">
-        <v>0</v>
+        <v>56</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1704,34 +1804,34 @@
         <v>16</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="H22" s="5" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J22" s="6">
-        <v>0</v>
-      </c>
-      <c r="K22" s="6">
-        <v>0</v>
+        <v>57</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1739,34 +1839,34 @@
         <v>17</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="6">
-        <v>0</v>
-      </c>
-      <c r="G23" s="6">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="K23" s="6">
-        <v>0</v>
+      <c r="K23" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1774,31 +1874,31 @@
         <v>18</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="6">
-        <v>0</v>
-      </c>
-      <c r="G24" s="6">
-        <v>0</v>
-      </c>
-      <c r="H24" s="6">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>44</v>
@@ -1841,37 +1941,36 @@
         <v>1</v>
       </c>
       <c r="B27" s="8">
-        <f>-B6*B8+1/2/B10</f>
-        <v>-3.217996698804695E-3</v>
+        <f>-B6*B8</f>
+        <v>-3.55760443637112E-3</v>
       </c>
       <c r="C27" s="8">
-        <f>1/2/B10</f>
-        <v>3.3960773756642489E-4</v>
-      </c>
-      <c r="D27" s="7">
-        <f>B6*B8+1/2/B10</f>
-        <v>3.8972121739375451E-3</v>
-      </c>
-      <c r="E27" s="7">
-        <f>-1/2/B10</f>
-        <v>-3.3960773756642489E-4</v>
-      </c>
-      <c r="F27" s="7">
-        <v>0</v>
-      </c>
-      <c r="G27" s="7">
-        <v>0</v>
-      </c>
-      <c r="H27" s="7">
-        <v>0</v>
-      </c>
-      <c r="I27" s="7">
-        <v>0</v>
-      </c>
-      <c r="J27" s="7">
-        <v>0</v>
-      </c>
-      <c r="K27" s="7">
+        <v>0</v>
+      </c>
+      <c r="D27" s="9">
+        <f>B6*B8+1/B10</f>
+        <v>4.2368199115039697E-3</v>
+      </c>
+      <c r="E27" s="9">
+        <f>-1/B10</f>
+        <v>-6.7921547513284978E-4</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+      <c r="H27" s="9">
+        <v>0</v>
+      </c>
+      <c r="I27" s="9">
+        <v>0</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0</v>
+      </c>
+      <c r="K27" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1880,37 +1979,37 @@
         <v>2</v>
       </c>
       <c r="B28" s="8">
-        <f>-1/2/B10</f>
-        <v>-3.3960773756642489E-4</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="C28" s="8">
-        <f>-B7*B9+1/2/B10+1/2/B11+1/2/B12</f>
-        <v>4.7682471112986473</v>
-      </c>
-      <c r="D28" s="7">
-        <f>-1/2/R_pipe</f>
-        <v>-3.3960773756642489E-4</v>
-      </c>
-      <c r="E28" s="7">
-        <f>m_a*Cp_a+1/2/R_pipe+1/2/R_int+1/2/R_ext</f>
-        <v>5.4914174737986459</v>
-      </c>
-      <c r="F28" s="7">
-        <v>0</v>
-      </c>
-      <c r="G28" s="7">
-        <v>0</v>
-      </c>
-      <c r="H28" s="7">
-        <v>0</v>
-      </c>
-      <c r="I28" s="7">
-        <v>0</v>
-      </c>
-      <c r="J28" s="7">
-        <v>0</v>
-      </c>
-      <c r="K28" s="7">
+        <f>-B7*B9</f>
+        <v>-0.36158518124999894</v>
+      </c>
+      <c r="D28" s="9">
+        <f>-1/R_pipe</f>
+        <v>-6.7921547513284978E-4</v>
+      </c>
+      <c r="E28" s="11">
+        <f>m_a*Cp_a+1/R_pipe+1/R_int+1/R_ext</f>
+        <v>10.621249766347292</v>
+      </c>
+      <c r="F28" s="9">
+        <v>0</v>
+      </c>
+      <c r="G28" s="9">
+        <v>0</v>
+      </c>
+      <c r="H28" s="9">
+        <v>0</v>
+      </c>
+      <c r="I28" s="9">
+        <v>0</v>
+      </c>
+      <c r="J28" s="9">
+        <v>0</v>
+      </c>
+      <c r="K28" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1924,30 +2023,30 @@
       <c r="C29" s="8">
         <v>0</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="9">
         <f>-m_w*Cp_w</f>
         <v>-3.55760443637112E-3</v>
       </c>
-      <c r="E29" s="7">
-        <v>0</v>
-      </c>
-      <c r="F29" s="7">
+      <c r="E29" s="9">
+        <v>0</v>
+      </c>
+      <c r="F29" s="9">
         <f>m_w*Cp_w</f>
         <v>3.55760443637112E-3</v>
       </c>
-      <c r="G29" s="7">
-        <v>0</v>
-      </c>
-      <c r="H29" s="7">
-        <v>0</v>
-      </c>
-      <c r="I29" s="7">
-        <v>0</v>
-      </c>
-      <c r="J29" s="7">
-        <v>0</v>
-      </c>
-      <c r="K29" s="7">
+      <c r="G29" s="9">
+        <v>0</v>
+      </c>
+      <c r="H29" s="9">
+        <v>0</v>
+      </c>
+      <c r="I29" s="9">
+        <v>0</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0</v>
+      </c>
+      <c r="K29" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1961,26 +2060,26 @@
       <c r="C30" s="8">
         <v>0</v>
       </c>
-      <c r="D30" s="7">
-        <v>0</v>
-      </c>
-      <c r="E30" s="7">
+      <c r="D30" s="9">
+        <v>0</v>
+      </c>
+      <c r="E30" s="9">
         <f>-m_a*Cp_a</f>
         <v>-0.36158518124999894</v>
       </c>
-      <c r="F30" s="7">
-        <v>0</v>
-      </c>
-      <c r="G30" s="7">
+      <c r="F30" s="9">
+        <v>0</v>
+      </c>
+      <c r="G30" s="9">
         <f>m_a*Cp_a</f>
         <v>0.36158518124999894</v>
       </c>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7">
-        <v>0</v>
-      </c>
-      <c r="K30" s="7">
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9">
+        <v>0</v>
+      </c>
+      <c r="K30" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1994,32 +2093,31 @@
       <c r="C31" s="8">
         <v>0</v>
       </c>
-      <c r="D31" s="7">
-        <v>0</v>
-      </c>
-      <c r="E31" s="7">
-        <v>0</v>
-      </c>
-      <c r="F31" s="7">
-        <f>-m_w*Cp_w+1/2/R_pipe</f>
-        <v>-3.217996698804695E-3</v>
-      </c>
-      <c r="G31" s="7">
-        <f>1/2/R_pipe</f>
-        <v>3.3960773756642489E-4</v>
-      </c>
-      <c r="H31" s="7">
-        <f>m_w*Cp_w+1/2/R_pipe</f>
-        <v>3.8972121739375451E-3</v>
-      </c>
-      <c r="I31" s="7">
-        <f>-1/2/R_pipe</f>
-        <v>-3.3960773756642489E-4</v>
-      </c>
-      <c r="J31" s="7">
-        <v>0</v>
-      </c>
-      <c r="K31" s="7">
+      <c r="D31" s="9">
+        <v>0</v>
+      </c>
+      <c r="E31" s="9">
+        <v>0</v>
+      </c>
+      <c r="F31" s="9">
+        <f>-m_w*Cp_w</f>
+        <v>-3.55760443637112E-3</v>
+      </c>
+      <c r="G31" s="9">
+        <v>0</v>
+      </c>
+      <c r="H31" s="9">
+        <f>m_w*Cp_w+1/R_pipe</f>
+        <v>4.2368199115039697E-3</v>
+      </c>
+      <c r="I31" s="9">
+        <f>-1/R_pipe</f>
+        <v>-6.7921547513284978E-4</v>
+      </c>
+      <c r="J31" s="9">
+        <v>0</v>
+      </c>
+      <c r="K31" s="9">
         <v>0</v>
       </c>
     </row>
@@ -2033,32 +2131,31 @@
       <c r="C32" s="8">
         <v>0</v>
       </c>
-      <c r="D32" s="7">
-        <v>0</v>
-      </c>
-      <c r="E32" s="7">
-        <v>0</v>
-      </c>
-      <c r="F32" s="7">
-        <f>-1/2/R_pipe</f>
-        <v>-3.3960773756642489E-4</v>
-      </c>
-      <c r="G32" s="7">
-        <f>-m_a*Cp_a+1/2/R_pipe+1/2/R_int+1/2/R_ext</f>
-        <v>4.7682471112986473</v>
-      </c>
-      <c r="H32" s="7">
-        <f>1/2/R_pipe</f>
-        <v>3.3960773756642489E-4</v>
-      </c>
-      <c r="I32" s="7">
-        <f>m_a*Cp_a+1/2/R_pipe+1/2/R_int+1/2/R_ext</f>
-        <v>5.4914174737986459</v>
-      </c>
-      <c r="J32" s="7">
-        <v>0</v>
-      </c>
-      <c r="K32" s="7">
+      <c r="D32" s="9">
+        <v>0</v>
+      </c>
+      <c r="E32" s="9">
+        <v>0</v>
+      </c>
+      <c r="F32" s="9">
+        <v>0</v>
+      </c>
+      <c r="G32" s="9">
+        <f>-m_a*Cp_a</f>
+        <v>-0.36158518124999894</v>
+      </c>
+      <c r="H32" s="9">
+        <f>1/R_pipe</f>
+        <v>6.7921547513284978E-4</v>
+      </c>
+      <c r="I32" s="11">
+        <f>m_a*Cp_a+1/R_pipe+1/R_int+1/R_ext</f>
+        <v>10.621249766347292</v>
+      </c>
+      <c r="J32" s="9">
+        <v>0</v>
+      </c>
+      <c r="K32" s="9">
         <v>0</v>
       </c>
     </row>
@@ -2072,30 +2169,30 @@
       <c r="C33" s="8">
         <v>0</v>
       </c>
-      <c r="D33" s="7">
-        <v>0</v>
-      </c>
-      <c r="E33" s="7">
-        <v>0</v>
-      </c>
-      <c r="F33" s="7">
-        <v>0</v>
-      </c>
-      <c r="G33" s="7">
-        <v>0</v>
-      </c>
-      <c r="H33" s="7">
+      <c r="D33" s="9">
+        <v>0</v>
+      </c>
+      <c r="E33" s="9">
+        <v>0</v>
+      </c>
+      <c r="F33" s="9">
+        <v>0</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0</v>
+      </c>
+      <c r="H33" s="9">
         <f>-m_w*Cp_w</f>
         <v>-3.55760443637112E-3</v>
       </c>
-      <c r="I33" s="7">
-        <v>0</v>
-      </c>
-      <c r="J33" s="7">
+      <c r="I33" s="9">
+        <v>0</v>
+      </c>
+      <c r="J33" s="9">
         <f>m_w*Cp_w</f>
         <v>3.55760443637112E-3</v>
       </c>
-      <c r="K33" s="7">
+      <c r="K33" s="9">
         <v>0</v>
       </c>
     </row>
@@ -2109,280 +2206,304 @@
       <c r="C34" s="8">
         <v>0</v>
       </c>
-      <c r="D34" s="7">
-        <v>0</v>
-      </c>
-      <c r="E34" s="7">
-        <v>0</v>
-      </c>
-      <c r="F34" s="7">
-        <v>0</v>
-      </c>
-      <c r="G34" s="7">
-        <v>0</v>
-      </c>
-      <c r="H34" s="7">
-        <v>0</v>
-      </c>
-      <c r="I34" s="7">
+      <c r="D34" s="9">
+        <v>0</v>
+      </c>
+      <c r="E34" s="9">
+        <v>0</v>
+      </c>
+      <c r="F34" s="9">
+        <v>0</v>
+      </c>
+      <c r="G34" s="9">
+        <v>0</v>
+      </c>
+      <c r="H34" s="9">
+        <v>0</v>
+      </c>
+      <c r="I34" s="9">
         <f>m_a*Cp_a</f>
         <v>0.36158518124999894</v>
       </c>
-      <c r="J34" s="7">
-        <v>0</v>
-      </c>
-      <c r="K34" s="7">
+      <c r="J34" s="9">
+        <v>0</v>
+      </c>
+      <c r="K34" s="9">
         <f>m_a*Cp_a</f>
         <v>0.36158518124999894</v>
       </c>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36">
+      <c r="A36" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="6">
         <f>m_w*Cp_w+1/2/R_pipe</f>
         <v>3.8972121739375451E-3</v>
       </c>
-      <c r="D36" s="9">
-        <v>3.8971565300000002E-3</v>
-      </c>
-      <c r="E36" s="9">
-        <v>-3.3960773799999999E-4</v>
-      </c>
-      <c r="F36" s="9">
-        <v>0</v>
-      </c>
-      <c r="G36" s="9">
-        <v>0</v>
-      </c>
-      <c r="H36" s="9">
-        <v>0</v>
-      </c>
-      <c r="I36" s="9">
-        <v>0</v>
-      </c>
-      <c r="J36" s="9">
-        <v>0</v>
-      </c>
-      <c r="K36" s="9">
+      <c r="C36" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="7">
+        <v>4.2329024999999999E-3</v>
+      </c>
+      <c r="E36" s="7">
+        <v>-6.7903105699999996E-4</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0</v>
+      </c>
+      <c r="G36" s="7">
+        <v>0</v>
+      </c>
+      <c r="H36" s="7">
+        <v>0</v>
+      </c>
+      <c r="I36" s="7">
+        <v>0</v>
+      </c>
+      <c r="J36" s="7">
+        <v>0</v>
+      </c>
+      <c r="K36" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" t="s">
-        <v>56</v>
-      </c>
-      <c r="B37">
+      <c r="A37" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="6">
         <f>-1/2/R_pipe</f>
         <v>-3.3960773756642489E-4</v>
       </c>
-      <c r="D37" s="9">
-        <v>-3.3960773799999999E-4</v>
-      </c>
-      <c r="E37" s="9">
-        <v>5.49141747</v>
-      </c>
-      <c r="F37" s="9">
-        <v>0</v>
-      </c>
-      <c r="G37" s="9">
-        <v>0</v>
-      </c>
-      <c r="H37" s="9">
-        <v>0</v>
-      </c>
-      <c r="I37" s="9">
-        <v>0</v>
-      </c>
-      <c r="J37" s="9">
-        <v>0</v>
-      </c>
-      <c r="K37" s="9">
+      <c r="C37" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="7">
+        <v>-6.7903105699999996E-4</v>
+      </c>
+      <c r="E37" s="7">
+        <v>10.109184300000001</v>
+      </c>
+      <c r="F37" s="7">
+        <v>0</v>
+      </c>
+      <c r="G37" s="7">
+        <v>0</v>
+      </c>
+      <c r="H37" s="7">
+        <v>0</v>
+      </c>
+      <c r="I37" s="7">
+        <v>0</v>
+      </c>
+      <c r="J37" s="7">
+        <v>0</v>
+      </c>
+      <c r="K37" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" t="s">
-        <v>57</v>
-      </c>
-      <c r="B38">
+      <c r="A38" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="6">
         <f>B2*(m_w*Cp_w-1/2/R_pipe)+B3*(1/2/R_pipe)</f>
         <v>4.8626111835789534E-2</v>
       </c>
-      <c r="D38" s="9">
-        <v>-3.5574554099999998E-3</v>
-      </c>
-      <c r="E38" s="9">
-        <v>0</v>
-      </c>
-      <c r="F38" s="9">
-        <v>3.5574554099999998E-3</v>
-      </c>
-      <c r="G38" s="9">
-        <v>0</v>
-      </c>
-      <c r="H38" s="9">
-        <v>0</v>
-      </c>
-      <c r="I38" s="9">
-        <v>0</v>
-      </c>
-      <c r="J38" s="9">
-        <v>0</v>
-      </c>
-      <c r="K38" s="9">
+      <c r="C38" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="7">
+        <v>-3.55203626E-3</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0</v>
+      </c>
+      <c r="F38" s="7">
+        <v>3.55203626E-3</v>
+      </c>
+      <c r="G38" s="7">
+        <v>0</v>
+      </c>
+      <c r="H38" s="7">
+        <v>0</v>
+      </c>
+      <c r="I38" s="7">
+        <v>0</v>
+      </c>
+      <c r="J38" s="7">
+        <v>0</v>
+      </c>
+      <c r="K38" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39">
+      <c r="A39" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="6">
         <f>-1/2/R_pipe</f>
         <v>-3.3960773756642489E-4</v>
       </c>
-      <c r="D39" s="9">
-        <v>0</v>
-      </c>
-      <c r="E39" s="9">
+      <c r="C39" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0</v>
+      </c>
+      <c r="E39" s="7">
         <v>-0.36158518099999998</v>
       </c>
-      <c r="F39" s="9">
-        <v>0</v>
-      </c>
-      <c r="G39" s="9">
+      <c r="F39" s="7">
+        <v>0</v>
+      </c>
+      <c r="G39" s="7">
         <v>0.36158518099999998</v>
       </c>
-      <c r="H39" s="9">
-        <v>0</v>
-      </c>
-      <c r="I39" s="9">
-        <v>0</v>
-      </c>
-      <c r="J39" s="9">
-        <v>0</v>
-      </c>
-      <c r="K39" s="9">
+      <c r="H39" s="7">
+        <v>0</v>
+      </c>
+      <c r="I39" s="7">
+        <v>0</v>
+      </c>
+      <c r="J39" s="7">
+        <v>0</v>
+      </c>
+      <c r="K39" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40">
+      <c r="A40" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="6">
         <f>m_a*Cp_a+1/2/R_pipe+1/2/R_int+1/2/R_ext</f>
         <v>5.4914174737986459</v>
       </c>
-      <c r="D40" s="9">
-        <v>0</v>
-      </c>
-      <c r="E40" s="9">
-        <v>0</v>
-      </c>
-      <c r="F40" s="9">
-        <v>-3.2177549900000001E-3</v>
-      </c>
-      <c r="G40" s="9">
-        <v>3.3960773799999999E-4</v>
-      </c>
-      <c r="H40" s="9">
-        <v>3.8969704699999999E-3</v>
-      </c>
-      <c r="I40" s="9">
-        <v>-3.3960773799999999E-4</v>
-      </c>
-      <c r="J40" s="9">
-        <v>0</v>
-      </c>
-      <c r="K40" s="9">
+      <c r="C40" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="7">
+        <v>0</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0</v>
+      </c>
+      <c r="F40" s="7">
+        <v>-3.55052502E-3</v>
+      </c>
+      <c r="G40" s="7">
+        <v>0</v>
+      </c>
+      <c r="H40" s="7">
+        <v>4.2295560800000003E-3</v>
+      </c>
+      <c r="I40" s="7">
+        <v>-6.7903105699999996E-4</v>
+      </c>
+      <c r="J40" s="7">
+        <v>0</v>
+      </c>
+      <c r="K40" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:11">
-      <c r="A41" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41">
+      <c r="A41" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="6">
         <f>B2*(1/2/R_pipe)+B3*(m_a*Cp_a-1/2/R_pipe-1/2/R_int-1/2/R_ext)+B4*(1/R_int)+B5*(1/R_ext)</f>
         <v>156.50047149302344</v>
       </c>
-      <c r="D41" s="9">
-        <v>0</v>
-      </c>
-      <c r="E41" s="9">
-        <v>0</v>
-      </c>
-      <c r="F41" s="9">
-        <v>-3.3960773799999999E-4</v>
-      </c>
-      <c r="G41" s="9">
-        <v>4.7682471099999999</v>
-      </c>
-      <c r="H41" s="9">
-        <v>-3.3960773799999999E-4</v>
-      </c>
-      <c r="I41" s="9">
-        <v>5.49141747</v>
-      </c>
-      <c r="J41" s="9">
-        <v>0</v>
-      </c>
-      <c r="K41" s="9">
+      <c r="C41" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="7">
+        <v>0</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0</v>
+      </c>
+      <c r="F41" s="7">
+        <v>0</v>
+      </c>
+      <c r="G41" s="7">
+        <v>-0.36158518099999998</v>
+      </c>
+      <c r="H41" s="7">
+        <v>-6.7903105699999996E-4</v>
+      </c>
+      <c r="I41" s="7">
+        <v>10.109184300000001</v>
+      </c>
+      <c r="J41" s="7">
+        <v>0</v>
+      </c>
+      <c r="K41" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:11">
-      <c r="D42" s="9">
-        <v>0</v>
-      </c>
-      <c r="E42" s="9">
-        <v>0</v>
-      </c>
-      <c r="F42" s="9">
-        <v>0</v>
-      </c>
-      <c r="G42" s="9">
-        <v>0</v>
-      </c>
-      <c r="H42" s="9">
-        <v>-3.55727075E-3</v>
-      </c>
-      <c r="I42" s="9">
-        <v>0</v>
-      </c>
-      <c r="J42" s="9">
-        <v>3.55727075E-3</v>
-      </c>
-      <c r="K42" s="9">
+      <c r="C42" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0</v>
+      </c>
+      <c r="E42" s="7">
+        <v>0</v>
+      </c>
+      <c r="F42" s="7">
+        <v>0</v>
+      </c>
+      <c r="G42" s="7">
+        <v>0</v>
+      </c>
+      <c r="H42" s="7">
+        <v>-3.5493003699999998E-3</v>
+      </c>
+      <c r="I42" s="7">
+        <v>0</v>
+      </c>
+      <c r="J42" s="7">
+        <v>3.5493003699999998E-3</v>
+      </c>
+      <c r="K42" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:11">
-      <c r="D43" s="9">
-        <v>0</v>
-      </c>
-      <c r="E43" s="9">
-        <v>0</v>
-      </c>
-      <c r="F43" s="9">
-        <v>0</v>
-      </c>
-      <c r="G43" s="9">
-        <v>0</v>
-      </c>
-      <c r="H43" s="9">
-        <v>0</v>
-      </c>
-      <c r="I43" s="9">
+      <c r="C43" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="7">
+        <v>0</v>
+      </c>
+      <c r="E43" s="7">
+        <v>0</v>
+      </c>
+      <c r="F43" s="7">
+        <v>0</v>
+      </c>
+      <c r="G43" s="7">
+        <v>0</v>
+      </c>
+      <c r="H43" s="7">
+        <v>0</v>
+      </c>
+      <c r="I43" s="7">
         <v>-0.36158518099999998</v>
       </c>
-      <c r="J43" s="9">
-        <v>0</v>
-      </c>
-      <c r="K43" s="9">
+      <c r="J43" s="7">
+        <v>0</v>
+      </c>
+      <c r="K43" s="7">
         <v>0.36158518099999998</v>
       </c>
     </row>

</xml_diff>

<commit_message>
20150108 - Fixed Sign at (8,5) and Moved Files
</commit_message>
<xml_diff>
--- a/Matrix Dependence.xlsx
+++ b/Matrix Dependence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-20" windowWidth="28800" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix by Hand" sheetId="2" r:id="rId1"/>
@@ -764,7 +764,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -774,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1545,8 +1545,8 @@
         <v>0</v>
       </c>
       <c r="I37" s="6">
-        <f>m_a*Cp_a</f>
-        <v>0.36158518124999894</v>
+        <f>-m_a*Cp_a</f>
+        <v>-0.36158518124999894</v>
       </c>
       <c r="J37" s="6">
         <v>0</v>

</xml_diff>

<commit_message>
20150108-Fixed Thermal Gen Units
Changed the generation to 0.008 kW instead of 8 kW. Fixed and solved
script crashing issues.
</commit_message>
<xml_diff>
--- a/Matrix Dependence.xlsx
+++ b/Matrix Dependence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17540"/>
+    <workbookView xWindow="-80" yWindow="-20" windowWidth="28800" windowHeight="17540" tabRatio="331"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix by Hand" sheetId="2" r:id="rId1"/>
@@ -262,7 +262,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,6 +305,16 @@
       <color indexed="206"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212121"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -418,7 +428,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -430,6 +440,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -764,7 +776,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -772,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:K46"/>
+  <dimension ref="A4:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1468,8 +1480,8 @@
         <v>-0.36158518124999894</v>
       </c>
       <c r="H35" s="6">
-        <f>1/R_pipe</f>
-        <v>6.7921547513284978E-4</v>
+        <f>-1/R_pipe</f>
+        <v>-6.7921547513284978E-4</v>
       </c>
       <c r="I35" s="8">
         <f>m_a*Cp_a+1/R_pipe+1/R_int+1/R_ext</f>
@@ -1827,6 +1839,214 @@
         <v>0</v>
       </c>
       <c r="K46" s="4">
+        <v>0.36158518099999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="D48" s="9">
+        <v>4.2368199999999996E-3</v>
+      </c>
+      <c r="E48" s="10">
+        <v>-6.7921500000000005E-4</v>
+      </c>
+      <c r="F48" s="10">
+        <v>0</v>
+      </c>
+      <c r="G48" s="10">
+        <v>0</v>
+      </c>
+      <c r="H48" s="10">
+        <v>0</v>
+      </c>
+      <c r="I48" s="10">
+        <v>0</v>
+      </c>
+      <c r="J48" s="10">
+        <v>0</v>
+      </c>
+      <c r="K48" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:11">
+      <c r="D49" s="9">
+        <v>-6.7921500000000005E-4</v>
+      </c>
+      <c r="E49" s="10">
+        <v>10.62124977</v>
+      </c>
+      <c r="F49" s="10">
+        <v>0</v>
+      </c>
+      <c r="G49" s="10">
+        <v>0</v>
+      </c>
+      <c r="H49" s="10">
+        <v>0</v>
+      </c>
+      <c r="I49" s="10">
+        <v>0</v>
+      </c>
+      <c r="J49" s="10">
+        <v>0</v>
+      </c>
+      <c r="K49" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:11">
+      <c r="D50" s="9">
+        <v>-3.5576039999999998E-3</v>
+      </c>
+      <c r="E50" s="10">
+        <v>0</v>
+      </c>
+      <c r="F50" s="10">
+        <v>3.5576039999999998E-3</v>
+      </c>
+      <c r="G50" s="10">
+        <v>0</v>
+      </c>
+      <c r="H50" s="10">
+        <v>0</v>
+      </c>
+      <c r="I50" s="10">
+        <v>0</v>
+      </c>
+      <c r="J50" s="10">
+        <v>0</v>
+      </c>
+      <c r="K50" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="4:11">
+      <c r="D51" s="9">
+        <v>0</v>
+      </c>
+      <c r="E51" s="10">
+        <v>-0.36158518099999998</v>
+      </c>
+      <c r="F51" s="10">
+        <v>0</v>
+      </c>
+      <c r="G51" s="10">
+        <v>0.36158518099999998</v>
+      </c>
+      <c r="H51" s="10">
+        <v>0</v>
+      </c>
+      <c r="I51" s="10">
+        <v>0</v>
+      </c>
+      <c r="J51" s="10">
+        <v>0</v>
+      </c>
+      <c r="K51" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="4:11">
+      <c r="D52" s="9">
+        <v>0</v>
+      </c>
+      <c r="E52" s="10">
+        <v>0</v>
+      </c>
+      <c r="F52" s="10">
+        <v>-3.5576039999999998E-3</v>
+      </c>
+      <c r="G52" s="10">
+        <v>0</v>
+      </c>
+      <c r="H52" s="10">
+        <v>4.2368199999999996E-3</v>
+      </c>
+      <c r="I52" s="10">
+        <v>-6.7921500000000005E-4</v>
+      </c>
+      <c r="J52" s="10">
+        <v>0</v>
+      </c>
+      <c r="K52" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="4:11">
+      <c r="D53" s="9">
+        <v>0</v>
+      </c>
+      <c r="E53" s="10">
+        <v>0</v>
+      </c>
+      <c r="F53" s="10">
+        <v>0</v>
+      </c>
+      <c r="G53" s="10">
+        <v>-0.36158518099999998</v>
+      </c>
+      <c r="H53" s="10">
+        <v>6.7921500000000005E-4</v>
+      </c>
+      <c r="I53" s="10">
+        <v>10.62124977</v>
+      </c>
+      <c r="J53" s="10">
+        <v>0</v>
+      </c>
+      <c r="K53" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="4:11">
+      <c r="D54" s="9">
+        <v>0</v>
+      </c>
+      <c r="E54" s="10">
+        <v>0</v>
+      </c>
+      <c r="F54" s="10">
+        <v>0</v>
+      </c>
+      <c r="G54" s="10">
+        <v>0</v>
+      </c>
+      <c r="H54" s="10">
+        <v>-3.5576039999999998E-3</v>
+      </c>
+      <c r="I54" s="10">
+        <v>0</v>
+      </c>
+      <c r="J54" s="10">
+        <v>3.5576039999999998E-3</v>
+      </c>
+      <c r="K54" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="4:11">
+      <c r="D55" s="9">
+        <v>0</v>
+      </c>
+      <c r="E55" s="10">
+        <v>0</v>
+      </c>
+      <c r="F55" s="10">
+        <v>0</v>
+      </c>
+      <c r="G55" s="10">
+        <v>0</v>
+      </c>
+      <c r="H55" s="10">
+        <v>0</v>
+      </c>
+      <c r="I55" s="10">
+        <v>-0.36158518099999998</v>
+      </c>
+      <c r="J55" s="10">
+        <v>0</v>
+      </c>
+      <c r="K55" s="10">
         <v>0.36158518099999998</v>
       </c>
     </row>

</xml_diff>